<commit_message>
Fixed spelling in the UI
</commit_message>
<xml_diff>
--- a/inputs/filters-and-indicators.xlsx
+++ b/inputs/filters-and-indicators.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
   <si>
     <t>README</t>
   </si>
@@ -130,12 +130,6 @@
     <t>For the Tea</t>
   </si>
   <si>
-    <t>They thought that</t>
-  </si>
-  <si>
-    <t>We were quitting</t>
-  </si>
-  <si>
     <t>Well when the sun went down</t>
   </si>
   <si>
@@ -329,6 +323,21 @@
   </si>
   <si>
     <t xml:space="preserve">She's a rapid </t>
+  </si>
+  <si>
+    <t>They thought</t>
+  </si>
+  <si>
+    <t>that we</t>
+  </si>
+  <si>
+    <t>Were quitting</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Added indicator info in</t>
   </si>
 </sst>
 </file>
@@ -835,7 +844,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -855,6 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1176,7 +1186,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1252,6 +1262,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="8">
+        <v>44267</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1260,7 +1284,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1315,13 +1339,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>21</v>
@@ -1335,13 +1359,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>21</v>
@@ -1355,13 +1379,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>21</v>
@@ -1373,13 +1397,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>21</v>
@@ -1393,13 +1417,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>21</v>
@@ -1413,13 +1437,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>21</v>
@@ -1433,13 +1457,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>21</v>
@@ -1451,21 +1475,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="10" t="s">
+    <row r="10" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>33</v>
@@ -1473,13 +1494,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>22</v>
@@ -1487,77 +1508,77 @@
       <c r="E11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>34</v>
+      <c r="F11" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="F12" s="11" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>36</v>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="C15" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>22</v>
@@ -1566,18 +1587,18 @@
         <v>23</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="C16" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>22</v>
@@ -1586,7 +1607,27 @@
         <v>23</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1611,10 +1652,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>15</v>
@@ -1625,142 +1666,142 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>